<commit_message>
Latest code from class 28 Feb
</commit_message>
<xml_diff>
--- a/HRMA/data/input.xlsx
+++ b/HRMA/data/input.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15570" windowHeight="6330"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15570" windowHeight="6330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="VerifyLoginLogout" sheetId="1" r:id="rId1"/>
+    <sheet name="Emp" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1:P19"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>UserName</t>
   </si>
@@ -39,13 +39,28 @@
   </si>
   <si>
     <t>login123</t>
+  </si>
+  <si>
+    <t>FN</t>
+  </si>
+  <si>
+    <t>LN</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,6 +122,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -185,6 +205,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -219,6 +240,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -394,21 +416,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -422,7 +444,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -440,4 +462,51 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>